<commit_message>
Updated EAC part in report, excel, slides
</commit_message>
<xml_diff>
--- a/6_Not_Capstone/Project.xlsx
+++ b/6_Not_Capstone/Project.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/capstone/6_Not_Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator2/Documents/GitHub/capstone/6_Not_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{374B6524-EBEE-7041-82B5-119BAE472F21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="11000" windowWidth="34480" windowHeight="22500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="440" windowWidth="25600" windowHeight="14460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Options Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Options for Report" sheetId="2" r:id="rId2"/>
     <sheet name="Present Worth" sheetId="4" r:id="rId3"/>
-    <sheet name="Present Worth (UK)" sheetId="6" r:id="rId4"/>
-    <sheet name="Incremental Rate of Return" sheetId="5" r:id="rId5"/>
-    <sheet name="Incremental Rate of Return (UK)" sheetId="8" r:id="rId6"/>
+    <sheet name="EAC" sheetId="9" r:id="rId4"/>
+    <sheet name="Present Worth (UK)" sheetId="6" r:id="rId5"/>
+    <sheet name="Incremental Rate of Return" sheetId="5" r:id="rId6"/>
+    <sheet name="Incremental Rate of Return (UK)" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="78">
   <si>
     <t>Option</t>
   </si>
@@ -196,16 +202,86 @@
   <si>
     <t>Energy Produced with diesel</t>
   </si>
+  <si>
+    <t>Wind Maintenance (2019)</t>
+  </si>
+  <si>
+    <t>Solar Maintenance (2019)</t>
+  </si>
+  <si>
+    <t>Diesel Maintenance (2019)</t>
+  </si>
+  <si>
+    <t>Diesel Fuel Cost (2019)</t>
+  </si>
+  <si>
+    <t>CO2 Output (kg in 2019)</t>
+  </si>
+  <si>
+    <t>EAC(capital cost)</t>
+  </si>
+  <si>
+    <t>EAC(maintnance)</t>
+  </si>
+  <si>
+    <t>EAC(operation) Diesel cost</t>
+  </si>
+  <si>
+    <t>EAC(operation) Carbon tax cost</t>
+  </si>
+  <si>
+    <t>EAC(total)</t>
+  </si>
+  <si>
+    <t>MARR before tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yearly maintnance cost raise </t>
+  </si>
+  <si>
+    <t>Yearly diesel cost raise (inflation)</t>
+  </si>
+  <si>
+    <t>Yearly CO2 output raise</t>
+  </si>
+  <si>
+    <t>Carbon tax rate / kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EAC (Solar + Wind + Diesel) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EAC (Diesel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EAC (Solar + Diesel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EAC (Wind + Diesel) </t>
+  </si>
+  <si>
+    <t>EAC = EAC(capital cost) + EAC(maintnance) + EAC(diesel cost) + EAC(CO2 tax cost)</t>
+  </si>
+  <si>
+    <t>i0 diesel inflation</t>
+  </si>
+  <si>
+    <t>i0 CO2 raise</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* ###0.00_);_(&quot;$&quot;* \(###0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,16 +319,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -262,25 +367,40 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -310,13 +430,35 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -333,9 +475,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -389,22 +531,22 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4999999999999999E-2</c:v>
+                  <c:v>-0.015</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.4999999999999998E-2</c:v>
+                  <c:v>-0.045</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7.4999999999999997E-2</c:v>
+                  <c:v>-0.075</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.09</c:v>
@@ -422,34 +564,34 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1134900650.7443235</c:v>
+                  <c:v>1.13490065074432E9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1097198388.6533368</c:v>
+                  <c:v>1.09719838865334E9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1059496126.56235</c:v>
+                  <c:v>1.05949612656235E9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1021793864.4713635</c:v>
+                  <c:v>1.02179386447136E9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>984091602.38037658</c:v>
+                  <c:v>9.84091602380377E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>946389340.28938985</c:v>
+                  <c:v>9.4638934028939E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>908687078.19840312</c:v>
+                  <c:v>9.08687078198403E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>870984816.10741615</c:v>
+                  <c:v>8.70984816107416E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2D7A-4F14-979B-C3E4778FDD23}"/>
             </c:ext>
@@ -492,34 +634,34 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>937760033.23974168</c:v>
+                  <c:v>9.37760033239742E8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>879891444.91404092</c:v>
+                  <c:v>8.79891444914041E8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>822022856.58834028</c:v>
+                  <c:v>8.2202285658834E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>764154268.26263976</c:v>
+                  <c:v>7.6415426826264E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>706285679.936939</c:v>
+                  <c:v>7.06285679936939E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>648417091.61123824</c:v>
+                  <c:v>6.48417091611238E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>590548503.2855376</c:v>
+                  <c:v>5.90548503285538E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>532679914.95983696</c:v>
+                  <c:v>5.32679914959837E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2D7A-4F14-979B-C3E4778FDD23}"/>
             </c:ext>
@@ -562,34 +704,34 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1397759018.7670934</c:v>
+                  <c:v>1.39775901876709E9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1387851215.0082994</c:v>
+                  <c:v>1.3878512150083E9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1377943411.2495055</c:v>
+                  <c:v>1.37794341124951E9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1368035607.490711</c:v>
+                  <c:v>1.36803560749071E9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1358127803.7319164</c:v>
+                  <c:v>1.35812780373192E9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1348219999.9731228</c:v>
+                  <c:v>1.34821999997312E9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1338312196.2143281</c:v>
+                  <c:v>1.33831219621433E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1328404392.4555342</c:v>
+                  <c:v>1.32840439245553E9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2D7A-4F14-979B-C3E4778FDD23}"/>
             </c:ext>
@@ -632,34 +774,34 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>856194795.15897357</c:v>
+                  <c:v>8.56194795158973E8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>786051051.73388183</c:v>
+                  <c:v>7.86051051733882E8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>715907308.30879021</c:v>
+                  <c:v>7.1590730830879E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>645763564.88369846</c:v>
+                  <c:v>6.45763564883698E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575619821.45860684</c:v>
+                  <c:v>5.75619821458607E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>505476078.0335151</c:v>
+                  <c:v>5.05476078033515E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>435332334.60842341</c:v>
+                  <c:v>4.35332334608423E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>365188591.18333173</c:v>
+                  <c:v>3.65188591183332E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-2D7A-4F14-979B-C3E4778FDD23}"/>
             </c:ext>
@@ -675,11 +817,1350 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="210063376"/>
-        <c:axId val="210064208"/>
+        <c:axId val="2099667168"/>
+        <c:axId val="-2121577232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="210063376"/>
+        <c:axId val="2099667168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Carbon Tax ($/kg-CO2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2121577232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2121577232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Present Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2099667168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Wind + Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>EAC!$B$26:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="_(&quot;$&quot;* ###0.00_);_(&quot;$&quot;* \(###0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EAC!$C$26:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.91627708546772E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.10904223648515E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Solar + Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>EAC!$D$26:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.43171997749009E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.14682134525798E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Solar + Wind + Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>EAC!$E$26:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.08021380965811E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.01667523658604E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>EAC!$F$26:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.59994682937492E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.67885757833205E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-2090567632"/>
+        <c:axId val="-2090090320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2090567632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* ###0.00_);_(&quot;$&quot;* \(###0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090090320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090090320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090567632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Wind+Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Present Worth (UK)'!$R$2:$Y$2</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.045</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.075</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Present Worth (UK)'!$R$23:$Y$23</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.09875935934112E9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06040879404503E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.02205822874895E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.83707663452867E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.45357098156784E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.07006532860701E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.68655967564618E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.30305402268535E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2C70-4592-97CA-FFC95B9F172E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Solar+Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Present Worth (UK)'!$R$47:$Y$47</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.97563252969438E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.38699594608008E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.79835936246579E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.20972277885149E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6210861952372E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0324496116229E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.44381302800861E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.85517644439431E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2C70-4592-97CA-FFC95B9F172E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Solar+Wind+Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Present Worth (UK)'!$R$71:$Y$71</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.36589507718364E9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35581690537328E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.34573873356291E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.33566056175254E9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.32558238994218E9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.31550421813181E9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.30542604632145E9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.29534787451108E9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2C70-4592-97CA-FFC95B9F172E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Diesel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Present Worth (UK)'!$R$95:$Y$95</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.19225542262937E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.47875653339992E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.76525764417047E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.05175875494102E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.33825986571157E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.62476097648213E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.91126208725268E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.19776319802323E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2C70-4592-97CA-FFC95B9F172E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2119502512"/>
+        <c:axId val="-2119754800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2119502512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +2258,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210064208"/>
+        <c:crossAx val="-2119754800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -785,7 +2266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210064208"/>
+        <c:axId val="-2119754800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,646 +2372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210063376"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Wind+Diesel</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Present Worth (UK)'!$R$2:$Y$2</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.4999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.03</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-4.4999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.06</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.4999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.09</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.105</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Present Worth (UK)'!$R$23:$Y$23</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1098759359.3411152</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1060408794.0450323</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1022058228.7489495</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>983707663.45286655</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>945357098.15678358</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>907006532.86070085</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>868655967.56461787</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>830305402.26853514</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C70-4592-97CA-FFC95B9F172E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Solar+Diesel</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Present Worth (UK)'!$R$47:$Y$47</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>897563252.96943796</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>838699594.60800827</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>779835936.24657905</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>720972277.88514912</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>662108619.52371979</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>603244961.16229022</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>544381302.80086076</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>485517644.43943113</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2C70-4592-97CA-FFC95B9F172E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Solar+Wind+Diesel</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Present Worth (UK)'!$R$71:$Y$71</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1365895077.183641</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1355816905.3732753</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1345738733.5629094</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1335660561.7525432</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1325582389.9421771</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1315504218.1318111</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1305426046.3214452</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1295347874.5110793</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2C70-4592-97CA-FFC95B9F172E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Diesel</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Present Worth (UK)'!$R$95:$Y$95</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>819225542.26293695</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>747875653.33999181</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>676525764.41704714</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>605175875.49410224</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>533825986.57115728</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>462476097.64821255</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>391126208.72526765</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>319776319.8023228</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2C70-4592-97CA-FFC95B9F172E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="210063376"/>
-        <c:axId val="210064208"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="210063376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Carbon Tax ($/kg-CO2)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="210064208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="210064208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total Present Value</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="210063376"/>
+        <c:crossAx val="-2119502512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1651,6 +2493,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2194,6 +3076,475 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2716,7 +4067,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2741,6 +4092,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2" title="EAC vs CO2 tax"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -2757,7 +4143,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2778,6 +4164,83 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Options Comparison"/>
+      <sheetName val="Options for Report"/>
+      <sheetName val="Present Worth"/>
+      <sheetName val="EAC"/>
+      <sheetName val="Present Worth (UK)"/>
+      <sheetName val="Incremental Rate of Return"/>
+      <sheetName val="Incremental Rate of Return (UK)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3">
+        <row r="24">
+          <cell r="B24">
+            <v>0</v>
+          </cell>
+          <cell r="C24">
+            <v>89302304.712497383</v>
+          </cell>
+          <cell r="D24">
+            <v>128037328.64260714</v>
+          </cell>
+          <cell r="E24">
+            <v>38210899.352686293</v>
+          </cell>
+          <cell r="F24">
+            <v>141649629.46043009</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>0.01</v>
+          </cell>
+          <cell r="C25">
+            <v>94199144.712497383</v>
+          </cell>
+          <cell r="D25">
+            <v>135553408.64260712</v>
+          </cell>
+          <cell r="E25">
+            <v>39497743.352686293</v>
+          </cell>
+          <cell r="F25">
+            <v>150760029.46043009</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>0.02</v>
+          </cell>
+          <cell r="C26">
+            <v>99095984.712497383</v>
+          </cell>
+          <cell r="D26">
+            <v>143069488.64260712</v>
+          </cell>
+          <cell r="E26">
+            <v>40784587.352686293</v>
+          </cell>
+          <cell r="F26">
+            <v>159870429.46043009</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3042,7 +4505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3105,11 +4568,11 @@
       <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -4911,7 +6374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5159,11 +6622,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J63" sqref="I63:J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11436,7 +12899,417 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11">
+        <v>94210000</v>
+      </c>
+      <c r="C2" s="11">
+        <v>100625000</v>
+      </c>
+      <c r="D2" s="11">
+        <v>96548000</v>
+      </c>
+      <c r="E2" s="11">
+        <v>56000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11">
+        <f>120*(1+$B$18)</f>
+        <v>126</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <f>120*(1+B18)</f>
+        <v>126</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="11">
+        <f>650*(1+B18)</f>
+        <v>682.5</v>
+      </c>
+      <c r="C5" s="11">
+        <f>720*(1+B18)</f>
+        <v>756</v>
+      </c>
+      <c r="D5" s="11">
+        <f>500*(1+B18)</f>
+        <v>525</v>
+      </c>
+      <c r="E5" s="11">
+        <f>1040*(1+$B$18)</f>
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="11">
+        <v>69954857.142857105</v>
+      </c>
+      <c r="C6" s="11">
+        <v>107372571.428571</v>
+      </c>
+      <c r="D6" s="11">
+        <v>18383485.714285702</v>
+      </c>
+      <c r="E6" s="11">
+        <v>130148571.428571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="16">
+        <v>489684000</v>
+      </c>
+      <c r="C7" s="16">
+        <v>751608000</v>
+      </c>
+      <c r="D7" s="16">
+        <v>128684400</v>
+      </c>
+      <c r="E7" s="16">
+        <v>911040000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="11">
+        <f>B7*$B$23</f>
+        <v>97936800</v>
+      </c>
+      <c r="C8" s="11">
+        <f>C7*$B$23</f>
+        <v>150321600</v>
+      </c>
+      <c r="D8" s="11">
+        <f>D7*$B$23</f>
+        <v>25736880</v>
+      </c>
+      <c r="E8" s="11">
+        <f>E7*$B$23</f>
+        <v>182208000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="11">
+        <f>B2*($B$17*(1+$B$17)^20)/((1+$B$17)^20-1)</f>
+        <v>19346638.756591562</v>
+      </c>
+      <c r="C9" s="11">
+        <f>C2*($B$17*(1+$B$17)^20)/((1+$B$17)^20-1)</f>
+        <v>20664000.900987428</v>
+      </c>
+      <c r="D9" s="11">
+        <f>D2*($B$17*(1+$B$17)^20)/((1+$B$17)^20-1)</f>
+        <v>19826762.325351894</v>
+      </c>
+      <c r="E9" s="11">
+        <f>E2*($B$17*(1+$B$17)^20)/((1+$B$17)^20-1)</f>
+        <v>11499965.718810396</v>
+      </c>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="11">
+        <f>SUM(B3:B5)+$B$18*(1/$B$17-20/(1+$B$17)^20-1)</f>
+        <v>808.67391594669539</v>
+      </c>
+      <c r="C10" s="11">
+        <f>SUM(C3:C5)+$B$18*(1/$B$17-20/(1+$B$17)^20-1)</f>
+        <v>756.17391594669539</v>
+      </c>
+      <c r="D10" s="11">
+        <f>SUM(D3:D5)+$B$18*(1/$B$17-20/(1+$B$17)^20-1)</f>
+        <v>651.17391594669539</v>
+      </c>
+      <c r="E10" s="11">
+        <f>SUM(E3:E5)+$B$18*(1/$B$17-20/(1+$B$17)^20-1)</f>
+        <v>1092.1739159466954</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="11">
+        <f>(B6*(((1+$B$20)^20-1)/($B$20*(1+$B$20)^20)*(1/1+$B$19)))*($B$17*($B$17+1)^20)/((1+$B$17)^20-1)</f>
+        <v>79815323.424169675</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" ref="C11:D11" si="0">(C6*(((1+$B$20)^20-1)/($B$20*(1+$B$20)^20)*(1/1+$B$19)))*($B$17*($B$17+1)^20)/((1+$B$17)^20-1)</f>
+        <v>122507240.60453908</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>20974724.527746912</v>
+      </c>
+      <c r="E11" s="11">
+        <f>(E6*(((1+$B$20)^20-1)/($B$20*(1+$B$20)^20)*(1/1+$B$19)))*($B$17*($B$17+1)^20)/((1+$B$17)^20-1)</f>
+        <v>148493624.97519898</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="11">
+        <f>(B8*(((1+$B$22)^20-1)/($B$22*(1+$B$22)^20)*(1/1+$B$21)))*($B$17*($B$17+1)^20)/((1+$B$17)^20-1)</f>
+        <v>111741452.79383761</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" ref="C12:E12" si="1">(C8*(((1+$B$22)^20-1)/($B$22*(1+$B$22)^20)*(1/1+$B$21)))*($B$17*($B$17+1)^20)/((1+$B$17)^20-1)</f>
+        <v>171510136.84635541</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
+        <v>29364614.338845696</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
+        <v>207891074.96527925</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="31">
+        <f>SUM(B9:B12)</f>
+        <v>210904223.64851481</v>
+      </c>
+      <c r="C13" s="31">
+        <f t="shared" ref="C13:E13" si="2">SUM(C9:C12)</f>
+        <v>314682134.52579784</v>
+      </c>
+      <c r="D13" s="31">
+        <f t="shared" si="2"/>
+        <v>70166752.365860447</v>
+      </c>
+      <c r="E13" s="31">
+        <f t="shared" si="2"/>
+        <v>367885757.83320457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="15">
+        <f>(1+$B$17)/(1+$B$19)-1</f>
+        <v>0.17647058823529416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="15">
+        <f>(1+$B$17)/(1+$B$21)-1</f>
+        <v>0.17647058823529416</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="34">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="35">
+        <v>0</v>
+      </c>
+      <c r="C26" s="34">
+        <v>99162770.854677185</v>
+      </c>
+      <c r="D26" s="34">
+        <v>143171997.74900883</v>
+      </c>
+      <c r="E26" s="34">
+        <v>40802138.096581124</v>
+      </c>
+      <c r="F26" s="34">
+        <v>159994682.93749169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="31">
+        <v>210904223.64851481</v>
+      </c>
+      <c r="D27" s="31">
+        <v>314682134.52579784</v>
+      </c>
+      <c r="E27" s="31">
+        <v>70166752.365860447</v>
+      </c>
+      <c r="F27" s="31">
+        <v>367885757.83320457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17673,8 +19546,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19553,7 +21426,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="26">
+      <c r="J51" s="25">
         <f>IRR(J30:J50)</f>
         <v>0.97473373744281511</v>
       </c>
@@ -20863,8 +22736,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEDF430-12F3-EF41-A436-9DC80868EB23}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22744,7 +24617,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="26">
+      <c r="J51" s="25">
         <f>IRR(J30:J50)</f>
         <v>0.97476171422699331</v>
       </c>

</xml_diff>